<commit_message>
RDM-4833 Move ids to the Page Object
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v13_RDM-4833_showandhide.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v13_RDM-4833_showandhide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9F3FB6-740D-7A41-8B95-7EE16AE8B3E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D929F88-32E1-4142-891B-425F8D64B6E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -3861,8 +3861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AD77"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView showGridLines="0" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6598,111 +6598,107 @@
       <c r="AB53" s="126"/>
       <c r="AC53" s="126"/>
     </row>
-    <row r="54" spans="1:29" s="138" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="133">
-        <v>42736</v>
-      </c>
-      <c r="B54" s="133"/>
-      <c r="C54" s="141" t="s">
+    <row r="54" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="123">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="123"/>
+      <c r="C54" s="124" t="s">
         <v>397</v>
       </c>
-      <c r="D54" s="141" t="s">
+      <c r="D54" s="124" t="s">
         <v>193</v>
       </c>
-      <c r="E54" s="134" t="s">
+      <c r="E54" s="125" t="s">
+        <v>494</v>
+      </c>
+      <c r="F54" s="126">
+        <v>3</v>
+      </c>
+      <c r="G54" s="124" t="s">
+        <v>218</v>
+      </c>
+      <c r="H54" s="124" t="s">
+        <v>402</v>
+      </c>
+      <c r="I54" s="124" t="s">
+        <v>399</v>
+      </c>
+      <c r="J54" s="127">
+        <v>1</v>
+      </c>
+      <c r="K54" s="126"/>
+      <c r="M54" s="126"/>
+      <c r="N54" s="124"/>
+      <c r="O54" s="129" t="s">
+        <v>195</v>
+      </c>
+      <c r="P54" s="126"/>
+      <c r="Q54" s="126"/>
+      <c r="R54" s="126"/>
+      <c r="S54" s="126"/>
+      <c r="T54" s="126"/>
+      <c r="U54" s="126"/>
+      <c r="V54" s="126"/>
+      <c r="W54" s="126"/>
+      <c r="X54" s="126"/>
+      <c r="Y54" s="126"/>
+      <c r="Z54" s="126"/>
+      <c r="AA54" s="126"/>
+      <c r="AB54" s="126"/>
+    </row>
+    <row r="55" spans="1:29" s="138" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="133">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="133"/>
+      <c r="C55" s="141" t="s">
+        <v>397</v>
+      </c>
+      <c r="D55" s="141" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="134" t="s">
         <v>333</v>
       </c>
-      <c r="F54" s="135">
+      <c r="F55" s="135">
         <v>11</v>
       </c>
-      <c r="G54" s="141" t="s">
+      <c r="G55" s="141" t="s">
         <v>218</v>
       </c>
-      <c r="H54" s="141" t="s">
+      <c r="H55" s="141" t="s">
         <v>402</v>
       </c>
-      <c r="I54" s="141" t="s">
+      <c r="I55" s="141" t="s">
         <v>399</v>
       </c>
-      <c r="J54" s="136">
+      <c r="J55" s="136">
         <v>1</v>
       </c>
-      <c r="K54" s="137"/>
-      <c r="L54" s="137" t="s">
+      <c r="K55" s="137"/>
+      <c r="L55" s="137" t="s">
         <v>400</v>
       </c>
-      <c r="M54" s="137"/>
-      <c r="N54" s="137"/>
-      <c r="O54" s="141" t="s">
+      <c r="M55" s="137"/>
+      <c r="N55" s="137"/>
+      <c r="O55" s="141" t="s">
         <v>195</v>
       </c>
-      <c r="P54" s="137"/>
-      <c r="Q54" s="137"/>
-      <c r="R54" s="137"/>
-      <c r="S54" s="137"/>
-      <c r="T54" s="137"/>
-      <c r="U54" s="137"/>
-      <c r="V54" s="137"/>
-      <c r="W54" s="137"/>
-      <c r="X54" s="137"/>
-      <c r="Y54" s="137"/>
-      <c r="Z54" s="137"/>
-      <c r="AA54" s="137"/>
-      <c r="AB54" s="137"/>
-      <c r="AC54" s="137"/>
-    </row>
-    <row r="55" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="123">
-        <v>42736</v>
-      </c>
-      <c r="B55" s="123"/>
-      <c r="C55" s="124" t="s">
-        <v>397</v>
-      </c>
-      <c r="D55" s="124" t="s">
-        <v>193</v>
-      </c>
-      <c r="E55" s="125" t="s">
-        <v>532</v>
-      </c>
-      <c r="F55" s="126">
-        <v>12</v>
-      </c>
-      <c r="G55" s="124" t="s">
-        <v>218</v>
-      </c>
-      <c r="H55" s="124" t="s">
-        <v>402</v>
-      </c>
-      <c r="I55" s="124" t="s">
-        <v>399</v>
-      </c>
-      <c r="J55" s="127">
-        <v>1</v>
-      </c>
-      <c r="K55" s="126"/>
-      <c r="L55" s="128" t="s">
-        <v>554</v>
-      </c>
-      <c r="M55" s="126"/>
-      <c r="N55" s="126"/>
-      <c r="O55" s="124" t="s">
-        <v>195</v>
-      </c>
-      <c r="P55" s="126"/>
-      <c r="Q55" s="126"/>
-      <c r="R55" s="126"/>
-      <c r="S55" s="126"/>
-      <c r="T55" s="126"/>
-      <c r="U55" s="126"/>
-      <c r="V55" s="126"/>
-      <c r="W55" s="126"/>
-      <c r="X55" s="126"/>
-      <c r="Y55" s="126"/>
-      <c r="Z55" s="126"/>
-      <c r="AA55" s="126"/>
-      <c r="AB55" s="126"/>
-      <c r="AC55" s="126"/>
+      <c r="P55" s="137"/>
+      <c r="Q55" s="137"/>
+      <c r="R55" s="137"/>
+      <c r="S55" s="137"/>
+      <c r="T55" s="137"/>
+      <c r="U55" s="137"/>
+      <c r="V55" s="137"/>
+      <c r="W55" s="137"/>
+      <c r="X55" s="137"/>
+      <c r="Y55" s="137"/>
+      <c r="Z55" s="137"/>
+      <c r="AA55" s="137"/>
+      <c r="AB55" s="137"/>
+      <c r="AC55" s="137"/>
     </row>
     <row r="56" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="123">
@@ -6716,10 +6712,10 @@
         <v>193</v>
       </c>
       <c r="E56" s="125" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F56" s="126">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G56" s="124" t="s">
         <v>218</v>
@@ -6735,7 +6731,7 @@
       </c>
       <c r="K56" s="126"/>
       <c r="L56" s="128" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="M56" s="126"/>
       <c r="N56" s="126"/>
@@ -6769,10 +6765,10 @@
         <v>193</v>
       </c>
       <c r="E57" s="125" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F57" s="126">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G57" s="124" t="s">
         <v>218</v>
@@ -6788,7 +6784,7 @@
       </c>
       <c r="K57" s="126"/>
       <c r="L57" s="128" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M57" s="126"/>
       <c r="N57" s="126"/>
@@ -6822,10 +6818,10 @@
         <v>193</v>
       </c>
       <c r="E58" s="125" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F58" s="126">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G58" s="124" t="s">
         <v>218</v>
@@ -6841,7 +6837,7 @@
       </c>
       <c r="K58" s="126"/>
       <c r="L58" s="128" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M58" s="126"/>
       <c r="N58" s="126"/>
@@ -6875,10 +6871,10 @@
         <v>193</v>
       </c>
       <c r="E59" s="125" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F59" s="126">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G59" s="124" t="s">
         <v>218</v>
@@ -6894,7 +6890,7 @@
       </c>
       <c r="K59" s="126"/>
       <c r="L59" s="128" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="M59" s="126"/>
       <c r="N59" s="126"/>
@@ -6928,10 +6924,10 @@
         <v>193</v>
       </c>
       <c r="E60" s="125" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F60" s="126">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G60" s="124" t="s">
         <v>218</v>
@@ -6947,7 +6943,7 @@
       </c>
       <c r="K60" s="126"/>
       <c r="L60" s="128" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M60" s="126"/>
       <c r="N60" s="126"/>
@@ -6981,10 +6977,10 @@
         <v>193</v>
       </c>
       <c r="E61" s="125" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F61" s="126">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G61" s="124" t="s">
         <v>218</v>
@@ -6999,8 +6995,8 @@
         <v>1</v>
       </c>
       <c r="K61" s="126"/>
-      <c r="L61" s="163" t="s">
-        <v>563</v>
+      <c r="L61" s="128" t="s">
+        <v>559</v>
       </c>
       <c r="M61" s="126"/>
       <c r="N61" s="126"/>
@@ -7034,10 +7030,10 @@
         <v>193</v>
       </c>
       <c r="E62" s="125" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F62" s="126">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G62" s="124" t="s">
         <v>218</v>
@@ -7052,8 +7048,8 @@
         <v>1</v>
       </c>
       <c r="K62" s="126"/>
-      <c r="L62" s="124" t="s">
-        <v>560</v>
+      <c r="L62" s="163" t="s">
+        <v>563</v>
       </c>
       <c r="M62" s="126"/>
       <c r="N62" s="126"/>
@@ -7087,10 +7083,10 @@
         <v>193</v>
       </c>
       <c r="E63" s="125" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F63" s="126">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G63" s="124" t="s">
         <v>218</v>
@@ -7106,7 +7102,7 @@
       </c>
       <c r="K63" s="126"/>
       <c r="L63" s="124" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="M63" s="126"/>
       <c r="N63" s="126"/>
@@ -7140,10 +7136,10 @@
         <v>193</v>
       </c>
       <c r="E64" s="125" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F64" s="126">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G64" s="124" t="s">
         <v>218</v>
@@ -7159,7 +7155,7 @@
       </c>
       <c r="K64" s="126"/>
       <c r="L64" s="124" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="M64" s="126"/>
       <c r="N64" s="126"/>
@@ -7181,158 +7177,162 @@
       <c r="AB64" s="126"/>
       <c r="AC64" s="126"/>
     </row>
-    <row r="65" spans="1:29" s="160" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="156">
-        <v>42736</v>
-      </c>
-      <c r="B65" s="156"/>
-      <c r="C65" s="157" t="s">
+    <row r="65" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="123">
+        <v>42736</v>
+      </c>
+      <c r="B65" s="123"/>
+      <c r="C65" s="124" t="s">
         <v>397</v>
       </c>
-      <c r="D65" s="157" t="s">
+      <c r="D65" s="124" t="s">
         <v>193</v>
       </c>
-      <c r="E65" s="158" t="s">
+      <c r="E65" s="125" t="s">
+        <v>550</v>
+      </c>
+      <c r="F65" s="126">
+        <v>25</v>
+      </c>
+      <c r="G65" s="124" t="s">
+        <v>218</v>
+      </c>
+      <c r="H65" s="124" t="s">
+        <v>402</v>
+      </c>
+      <c r="I65" s="124" t="s">
+        <v>399</v>
+      </c>
+      <c r="J65" s="127">
+        <v>1</v>
+      </c>
+      <c r="K65" s="126"/>
+      <c r="L65" s="124" t="s">
+        <v>562</v>
+      </c>
+      <c r="M65" s="126"/>
+      <c r="N65" s="126"/>
+      <c r="O65" s="124" t="s">
+        <v>195</v>
+      </c>
+      <c r="P65" s="126"/>
+      <c r="Q65" s="126"/>
+      <c r="R65" s="126"/>
+      <c r="S65" s="126"/>
+      <c r="T65" s="126"/>
+      <c r="U65" s="126"/>
+      <c r="V65" s="126"/>
+      <c r="W65" s="126"/>
+      <c r="X65" s="126"/>
+      <c r="Y65" s="126"/>
+      <c r="Z65" s="126"/>
+      <c r="AA65" s="126"/>
+      <c r="AB65" s="126"/>
+      <c r="AC65" s="126"/>
+    </row>
+    <row r="66" spans="1:29" s="160" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="156">
+        <v>42736</v>
+      </c>
+      <c r="B66" s="156"/>
+      <c r="C66" s="157" t="s">
+        <v>397</v>
+      </c>
+      <c r="D66" s="157" t="s">
+        <v>193</v>
+      </c>
+      <c r="E66" s="158" t="s">
         <v>567</v>
       </c>
-      <c r="F65" s="159">
+      <c r="F66" s="159">
         <v>26</v>
       </c>
-      <c r="G65" s="157" t="s">
+      <c r="G66" s="157" t="s">
         <v>218</v>
       </c>
-      <c r="H65" s="157" t="s">
+      <c r="H66" s="157" t="s">
         <v>402</v>
       </c>
-      <c r="I65" s="157" t="s">
+      <c r="I66" s="157" t="s">
         <v>399</v>
       </c>
-      <c r="J65" s="162">
+      <c r="J66" s="162">
         <v>1</v>
       </c>
-      <c r="K65" s="159"/>
-      <c r="L65" s="184" t="s">
+      <c r="K66" s="159"/>
+      <c r="L66" s="184" t="s">
         <v>566</v>
       </c>
-      <c r="M65" s="159"/>
-      <c r="N65" s="159"/>
-      <c r="O65" s="157"/>
-      <c r="P65" s="159"/>
-      <c r="Q65" s="159"/>
-      <c r="R65" s="159"/>
-      <c r="S65" s="159"/>
-      <c r="T65" s="159"/>
-      <c r="U65" s="159"/>
-      <c r="V65" s="159"/>
-      <c r="W65" s="159"/>
-      <c r="X65" s="159"/>
-      <c r="Y65" s="159"/>
-      <c r="Z65" s="159"/>
-      <c r="AA65" s="159"/>
-      <c r="AB65" s="159"/>
-      <c r="AC65" s="159"/>
-    </row>
-    <row r="66" spans="1:29" s="138" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="133">
-        <v>42736</v>
-      </c>
-      <c r="B66" s="133"/>
-      <c r="C66" s="141" t="s">
+      <c r="M66" s="159"/>
+      <c r="N66" s="159"/>
+      <c r="O66" s="157"/>
+      <c r="P66" s="159"/>
+      <c r="Q66" s="159"/>
+      <c r="R66" s="159"/>
+      <c r="S66" s="159"/>
+      <c r="T66" s="159"/>
+      <c r="U66" s="159"/>
+      <c r="V66" s="159"/>
+      <c r="W66" s="159"/>
+      <c r="X66" s="159"/>
+      <c r="Y66" s="159"/>
+      <c r="Z66" s="159"/>
+      <c r="AA66" s="159"/>
+      <c r="AB66" s="159"/>
+      <c r="AC66" s="159"/>
+    </row>
+    <row r="67" spans="1:29" s="138" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="133">
+        <v>42736</v>
+      </c>
+      <c r="B67" s="133"/>
+      <c r="C67" s="141" t="s">
         <v>397</v>
       </c>
-      <c r="D66" s="141" t="s">
+      <c r="D67" s="141" t="s">
         <v>193</v>
       </c>
-      <c r="E66" s="134" t="s">
+      <c r="E67" s="134" t="s">
         <v>336</v>
       </c>
-      <c r="F66" s="135">
+      <c r="F67" s="135">
         <v>1</v>
       </c>
-      <c r="G66" s="141" t="s">
+      <c r="G67" s="141" t="s">
         <v>218</v>
       </c>
-      <c r="H66" s="141" t="s">
+      <c r="H67" s="141" t="s">
         <v>403</v>
       </c>
-      <c r="I66" s="141" t="s">
+      <c r="I67" s="141" t="s">
         <v>401</v>
       </c>
-      <c r="J66" s="136">
+      <c r="J67" s="136">
         <v>2</v>
       </c>
-      <c r="K66" s="137"/>
-      <c r="L66" s="140"/>
-      <c r="M66" s="137" t="s">
+      <c r="K67" s="137"/>
+      <c r="L67" s="140"/>
+      <c r="M67" s="137" t="s">
         <v>400</v>
       </c>
-      <c r="N66" s="137"/>
-      <c r="O66" s="141" t="s">
+      <c r="N67" s="137"/>
+      <c r="O67" s="141" t="s">
         <v>195</v>
       </c>
-      <c r="P66" s="137"/>
-      <c r="Q66" s="137"/>
-      <c r="R66" s="137"/>
-      <c r="S66" s="137"/>
-      <c r="T66" s="137"/>
-      <c r="U66" s="137"/>
-      <c r="V66" s="137"/>
-      <c r="W66" s="137"/>
-      <c r="X66" s="137"/>
-      <c r="Y66" s="137"/>
-      <c r="Z66" s="137"/>
-      <c r="AA66" s="137"/>
-      <c r="AB66" s="137"/>
-      <c r="AC66" s="137"/>
-    </row>
-    <row r="67" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="123">
-        <v>42736</v>
-      </c>
-      <c r="B67" s="123"/>
-      <c r="C67" s="124" t="s">
-        <v>397</v>
-      </c>
-      <c r="D67" s="124" t="s">
-        <v>193</v>
-      </c>
-      <c r="E67" s="125" t="s">
-        <v>494</v>
-      </c>
-      <c r="F67" s="126">
-        <v>3</v>
-      </c>
-      <c r="G67" s="124" t="s">
-        <v>218</v>
-      </c>
-      <c r="H67" s="124" t="s">
-        <v>402</v>
-      </c>
-      <c r="I67" s="124" t="s">
-        <v>399</v>
-      </c>
-      <c r="J67" s="127">
-        <v>1</v>
-      </c>
-      <c r="K67" s="126"/>
-      <c r="M67" s="126"/>
-      <c r="N67" s="124"/>
-      <c r="O67" s="129" t="s">
-        <v>195</v>
-      </c>
-      <c r="P67" s="126"/>
-      <c r="Q67" s="126"/>
-      <c r="R67" s="126"/>
-      <c r="S67" s="126"/>
-      <c r="T67" s="126"/>
-      <c r="U67" s="126"/>
-      <c r="V67" s="126"/>
-      <c r="W67" s="126"/>
-      <c r="X67" s="126"/>
-      <c r="Y67" s="126"/>
-      <c r="Z67" s="126"/>
-      <c r="AA67" s="126"/>
-      <c r="AB67" s="126"/>
+      <c r="P67" s="137"/>
+      <c r="Q67" s="137"/>
+      <c r="R67" s="137"/>
+      <c r="S67" s="137"/>
+      <c r="T67" s="137"/>
+      <c r="U67" s="137"/>
+      <c r="V67" s="137"/>
+      <c r="W67" s="137"/>
+      <c r="X67" s="137"/>
+      <c r="Y67" s="137"/>
+      <c r="Z67" s="137"/>
+      <c r="AA67" s="137"/>
+      <c r="AB67" s="137"/>
+      <c r="AC67" s="137"/>
     </row>
     <row r="68" spans="1:29" s="128" customFormat="1" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="123">
@@ -11754,7 +11754,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12943,8 +12943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV77"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -24065,7 +24065,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25544,8 +25544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E561A8A-480D-6D45-8F14-5D4A9428A511}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>